<commit_message>
factor(xlspython_factorise): adapt filesave, checklinenumber, extractcoltabs, gathercolumn, extractcelltabs, stringinbinary, cpcolumnontabs, cpcellontabs, mergecells, convertminutes, groupofanswers, colorcasescolumn, colorcasestab, colorlines, cutstring, delete commands, columnbyqcmanswer, maptwocols, colgetpart, colcongruent, maxnames, gathermultianswers
</commit_message>
<xml_diff>
--- a/fichiers_xls/dataset.xlsx
+++ b/fichiers_xls/dataset.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ref" sheetId="1" state="visible" r:id="rId1"/>
@@ -275,8 +275,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:C6 A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:C6"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:C6"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C2:C6 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -560,8 +560,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:C6"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
feat(xlspython): modify extract_cells_from_all_tabs, addcolumn, maxnames, cpcolumnontabs, cpcellontabs method to use StringExtractor.
</commit_message>
<xml_diff>
--- a/fichiers_xls/dataset.xlsx
+++ b/fichiers_xls/dataset.xlsx
@@ -276,7 +276,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C6"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -347,6 +347,8 @@
         <v/>
       </c>
     </row>
+    <row r="7" ht="12.75" customHeight="1" s="2"/>
+    <row r="8" ht="12.75" customHeight="1" s="2"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -371,7 +373,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C6"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -381,11 +383,11 @@
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <f>A2+A3</f>
         <v/>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <f>B2+B3</f>
         <v/>
       </c>
@@ -394,11 +396,11 @@
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <f>A3+A4</f>
         <v/>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <f>B3+B4</f>
         <v/>
       </c>
@@ -407,11 +409,11 @@
       <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <f>A4+A5</f>
         <v/>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <f>B4+B5</f>
         <v/>
       </c>
@@ -420,11 +422,11 @@
       <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <f>A5+A6</f>
         <v/>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <f>B5+B6</f>
         <v/>
       </c>
@@ -433,11 +435,11 @@
       <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <f>A6+A7</f>
         <v/>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <f>B6+B7</f>
         <v/>
       </c>
@@ -466,7 +468,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C2:C6 C1"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -476,11 +478,11 @@
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <f>A2+A3</f>
         <v/>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <f>B2+B3</f>
         <v/>
       </c>
@@ -489,11 +491,11 @@
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <f>A3+A4</f>
         <v/>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <f>B3+B4</f>
         <v/>
       </c>
@@ -502,11 +504,11 @@
       <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <f>A4+A5</f>
         <v/>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <f>B4+B5</f>
         <v/>
       </c>
@@ -515,11 +517,11 @@
       <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <f>A5+A6</f>
         <v/>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <f>B5+B6</f>
         <v/>
       </c>
@@ -528,11 +530,11 @@
       <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <f>A6+A7</f>
         <v/>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <f>B6+B7</f>
         <v/>
       </c>
@@ -561,7 +563,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C6"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -571,11 +573,11 @@
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <f>A2+A3</f>
         <v/>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <f>B2+B3</f>
         <v/>
       </c>
@@ -584,11 +586,11 @@
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <f>A3+A4</f>
         <v/>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <f>B3+B4</f>
         <v/>
       </c>
@@ -597,11 +599,11 @@
       <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <f>A4+A5</f>
         <v/>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <f>B4+B5</f>
         <v/>
       </c>
@@ -610,11 +612,11 @@
       <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <f>A5+A6</f>
         <v/>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <f>B5+B6</f>
         <v/>
       </c>
@@ -623,11 +625,11 @@
       <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <f>A6+A7</f>
         <v/>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <f>B6+B7</f>
         <v/>
       </c>

</xml_diff>